<commit_message>
Update with Dec 2024 data
</commit_message>
<xml_diff>
--- a/data/cumulative_es_rules/cumulative_econ_significant_rules_by_presidential_month.xlsx
+++ b/data/cumulative_es_rules/cumulative_econ_significant_rules_by_presidential_month.xlsx
@@ -1964,7 +1964,9 @@
       <c r="H49" t="n">
         <v>226</v>
       </c>
-      <c r="I49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>310</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">

</xml_diff>